<commit_message>
add aws tag array
</commit_message>
<xml_diff>
--- a/spec/files/0_3_5_multiple_measure_paths.xlsx
+++ b/spec/files/0_3_5_multiple_measure_paths.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="837">
   <si>
     <t>type</t>
   </si>
@@ -2543,6 +2543,15 @@
   </si>
   <si>
     <t>../../spec/files/measures_second_path</t>
+  </si>
+  <si>
+    <t>AWS Tag</t>
+  </si>
+  <si>
+    <t>org=5500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nothing=else matters       </t>
   </si>
 </sst>
 </file>
@@ -2679,8 +2688,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1767">
+  <cellStyleXfs count="1769">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4564,7 +4575,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1767">
+  <cellStyles count="1769">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5448,6 +5459,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1762" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1764" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1768" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6331,6 +6343,7 @@
     <cellStyle name="Hyperlink" xfId="1761" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1763" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1767" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6664,10 +6677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6793,85 +6806,85 @@
         <v>608</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="12" customFormat="1">
-      <c r="A11" s="11" t="s">
+    <row r="10" spans="1:5" s="30" customFormat="1">
+      <c r="A10" s="30" t="s">
+        <v>834</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>835</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" s="30" customFormat="1">
+      <c r="A11" s="30" t="s">
+        <v>834</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>836</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="13" spans="1:5" s="12" customFormat="1">
+      <c r="A13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B14" s="24" t="s">
         <v>810</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>472</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>811</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="30" customFormat="1">
-      <c r="A14" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>833</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="30" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="B16" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>438</v>
+        <v>811</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="30" customFormat="1">
+      <c r="A16" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>833</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="30" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="B17" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>610</v>
+        <v>26</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>466</v>
+        <v>463</v>
+      </c>
+      <c r="B18" s="25" t="b">
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>438</v>
@@ -6879,290 +6892,312 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B19" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>466</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B21" s="24" t="s">
         <v>557</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A21" s="11" t="s">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>611</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="13" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="13" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B24" s="24" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="30" customFormat="1">
-      <c r="B23" s="25"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:5" s="30" customFormat="1">
+      <c r="B25" s="25"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A26" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>614</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>612</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>613</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="30" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="30" t="s">
         <v>572</v>
       </c>
-      <c r="B25" s="25" t="str">
-        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+      <c r="B27" s="25" t="str">
+        <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v>individual_variables</v>
       </c>
-      <c r="C25" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+      <c r="C27" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D27" s="34" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+    <row r="28" spans="1:5">
+      <c r="A28" s="30" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
-      <c r="B26" s="25" t="str">
-        <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+      <c r="B28" s="25" t="str">
+        <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C26" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+      <c r="C28" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="30" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
-      <c r="B27" s="25" t="str">
-        <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+      <c r="B29" s="25" t="str">
+        <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C27" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
-        <v/>
-      </c>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:5" s="30" customFormat="1">
-      <c r="A28" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
-        <v/>
-      </c>
-      <c r="B28" s="25" t="str">
-        <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
-        <v/>
-      </c>
-      <c r="C28" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
-        <v/>
-      </c>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:5" s="30" customFormat="1">
-      <c r="A29" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
-        <v/>
-      </c>
-      <c r="B29" s="25" t="str">
-        <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
-        <v/>
-      </c>
       <c r="C29" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:5" s="30" customFormat="1">
       <c r="A30" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B30" s="25" t="str">
-        <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C30" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D30" s="34"/>
     </row>
     <row r="31" spans="1:5" s="30" customFormat="1">
       <c r="A31" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B31" s="25" t="str">
-        <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C31" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:5" s="30" customFormat="1">
       <c r="A32" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B32" s="25" t="str">
-        <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C32" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D32" s="34"/>
     </row>
     <row r="33" spans="1:5" s="30" customFormat="1">
       <c r="A33" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B33" s="25" t="str">
-        <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C33" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D33" s="34"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" s="30" customFormat="1">
       <c r="A34" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B34" s="25" t="str">
-        <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C34" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:5" s="30" customFormat="1">
       <c r="A35" s="30" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
         <v/>
       </c>
       <c r="B35" s="25" t="str">
-        <f>IF(D35&lt;&gt;"",D35,IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)-1)))</f>
+        <f>IF(D35&lt;&gt;"",D35,IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
       <c r="C35" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B22,Lookups!$A$17:$A$23,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
       <c r="D35" s="34"/>
     </row>
-    <row r="36" spans="1:5" s="30" customFormat="1">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A37" s="11" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="30" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
+        <v/>
+      </c>
+      <c r="B36" s="25" t="str">
+        <f>IF(D36&lt;&gt;"",D36,IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
+        <v/>
+      </c>
+      <c r="C36" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
+        <v/>
+      </c>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:5" s="30" customFormat="1">
+      <c r="A37" s="30" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-2))</f>
+        <v/>
+      </c>
+      <c r="B37" s="25" t="str">
+        <f>IF(D37&lt;&gt;"",D37,IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)-1)))</f>
+        <v/>
+      </c>
+      <c r="C37" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B24,Lookups!$A$17:$A$23,0)))</f>
+        <v/>
+      </c>
+      <c r="D37" s="34"/>
+    </row>
+    <row r="38" spans="1:5" s="30" customFormat="1">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B39" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
+      <c r="D39" s="11"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B40" s="53" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A40" s="11" t="s">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A42" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B42" s="26" t="s">
         <v>454</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E42" s="13" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="30" customFormat="1">
-      <c r="A41" s="30" t="s">
+    <row r="43" spans="1:5" s="30" customFormat="1">
+      <c r="A43" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C43" s="30" t="s">
         <v>814</v>
       </c>
-      <c r="D41" s="54" t="s">
+      <c r="D43" s="54" t="s">
         <v>813</v>
       </c>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A43" s="11" t="s">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B45" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>615</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="13" t="s">
+      <c r="D45" s="11"/>
+      <c r="E45" s="13" t="s">
         <v>616</v>
       </c>
     </row>
@@ -7171,13 +7206,13 @@
     <sortCondition ref="B40"/>
   </sortState>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
       <formula1>AnalysisType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
       <formula1>TrueFalse</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
       <formula1>simulate_data_point</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:B8">

</xml_diff>

<commit_message>
add more checks on measure path test
</commit_message>
<xml_diff>
--- a/spec/files/0_3_5_multiple_measure_paths.xlsx
+++ b/spec/files/0_3_5_multiple_measure_paths.xlsx
@@ -1900,9 +1900,6 @@
     <t xml:space="preserve"> - Worker Only - </t>
   </si>
   <si>
-    <t>1.6.1</t>
-  </si>
-  <si>
     <t>Delta X</t>
   </si>
   <si>
@@ -2494,9 +2491,6 @@
     <t>Short Display Name</t>
   </si>
   <si>
-    <t>0.3.3</t>
-  </si>
-  <si>
     <t>Short display names are used for plots and exported to metadata</t>
   </si>
   <si>
@@ -2552,6 +2546,12 @@
   </si>
   <si>
     <t xml:space="preserve">nothing=else matters       </t>
+  </si>
+  <si>
+    <t>0.3.5</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
   </si>
 </sst>
 </file>
@@ -6680,7 +6680,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6716,7 +6716,7 @@
         <v>437</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>817</v>
+        <v>835</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>438</v>
@@ -6738,7 +6738,7 @@
         <v>470</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>619</v>
+        <v>836</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>617</v>
@@ -6749,7 +6749,7 @@
         <v>471</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>473</v>
@@ -6808,10 +6808,10 @@
     </row>
     <row r="10" spans="1:5" s="30" customFormat="1">
       <c r="A10" s="30" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="32"/>
@@ -6819,10 +6819,10 @@
     </row>
     <row r="11" spans="1:5" s="30" customFormat="1">
       <c r="A11" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>834</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>836</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="32"/>
@@ -6842,7 +6842,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>472</v>
@@ -6853,10 +6853,10 @@
         <v>25</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="30" customFormat="1">
@@ -6864,11 +6864,11 @@
         <v>25</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="30" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6876,7 +6876,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7154,7 +7154,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
@@ -7179,10 +7179,10 @@
         <v>32</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D43" s="54" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E43" s="2"/>
     </row>
@@ -7336,7 +7336,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G3" s="52" t="s">
         <v>11</v>
@@ -7363,7 +7363,7 @@
         <v>9</v>
       </c>
       <c r="O3" s="52" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="P3" s="52" t="s">
         <v>476</v>
@@ -7396,7 +7396,7 @@
         <v>19</v>
       </c>
       <c r="AB3" s="51" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="40" customFormat="1">
@@ -7427,19 +7427,19 @@
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>76</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I5" s="45">
         <v>0</v>
@@ -7459,7 +7459,7 @@
         <v>59.833333333333336</v>
       </c>
       <c r="R5" s="44" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S5" s="44"/>
     </row>
@@ -7468,10 +7468,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>69</v>
@@ -7484,13 +7484,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
+        <v>638</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>825</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>639</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>827</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>640</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>161</v>
@@ -7505,19 +7505,19 @@
         <v>21</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F8" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>826</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>828</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -7873,10 +7873,10 @@
         <v>460</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>461</v>
@@ -7888,40 +7888,40 @@
         <v>11</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="14" t="s">
         <v>646</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>647</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>648</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>649</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="14" customFormat="1" ht="30">
       <c r="A3" s="14" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>462</v>
@@ -7933,27 +7933,27 @@
         <v>462</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="29" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>469</v>
@@ -7976,16 +7976,16 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="29" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>469</v>
@@ -8015,16 +8015,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="29" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>469</v>
@@ -8047,16 +8047,16 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="29" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>469</v>
@@ -8079,15 +8079,15 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="29" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>65</v>
@@ -8108,15 +8108,15 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="29" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>65</v>
@@ -8137,17 +8137,17 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="29" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>65</v>
@@ -8168,15 +8168,15 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="29" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>65</v>
@@ -8197,12 +8197,12 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="29" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>469</v>
@@ -8226,12 +8226,12 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="29" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>469</v>
@@ -8255,12 +8255,12 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="29" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>469</v>
@@ -8284,12 +8284,12 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="29" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>469</v>
@@ -8313,12 +8313,12 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="29" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>469</v>
@@ -8342,12 +8342,12 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="29" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>469</v>
@@ -8371,12 +8371,12 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="29" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>469</v>
@@ -8400,12 +8400,12 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="29" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>469</v>
@@ -8429,12 +8429,12 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="29" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>469</v>
@@ -8458,12 +8458,12 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>469</v>
@@ -8487,12 +8487,12 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="29" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>469</v>
@@ -8516,12 +8516,12 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="29" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>469</v>
@@ -8545,12 +8545,12 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>469</v>
@@ -8574,12 +8574,12 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
       <c r="D25" s="29" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>469</v>
@@ -8603,15 +8603,15 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>65</v>
@@ -8632,15 +8632,15 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>65</v>
@@ -8661,17 +8661,17 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>65</v>
@@ -8692,15 +8692,15 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="29" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>65</v>
@@ -8721,15 +8721,15 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="29" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>65</v>
@@ -8750,15 +8750,15 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>66</v>
@@ -8779,15 +8779,15 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>65</v>
@@ -8808,17 +8808,17 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="29" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B33" s="29"/>
       <c r="C33" s="29" t="s">
+        <v>682</v>
+      </c>
+      <c r="D33" s="29" t="s">
         <v>683</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>684</v>
-      </c>
       <c r="E33" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>65</v>
@@ -8839,15 +8839,15 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="29" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>65</v>
@@ -8868,17 +8868,17 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>66</v>
@@ -8899,17 +8899,17 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B36" s="29"/>
       <c r="C36" s="29" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>65</v>
@@ -8930,13 +8930,13 @@
     </row>
     <row r="37" spans="1:13" s="29" customFormat="1">
       <c r="A37" s="29" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>65</v>
@@ -8955,13 +8955,13 @@
     </row>
     <row r="38" spans="1:13" s="29" customFormat="1">
       <c r="A38" s="29" t="s">
+        <v>688</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>689</v>
       </c>
-      <c r="D38" s="29" t="s">
-        <v>690</v>
-      </c>
       <c r="E38" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F38" s="29" t="s">
         <v>65</v>
@@ -8980,15 +8980,15 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>65</v>
@@ -9006,15 +9006,15 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F40" s="29" t="s">
         <v>65</v>
@@ -9032,15 +9032,15 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="29" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
       <c r="D41" s="29" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F41" s="29" t="s">
         <v>65</v>
@@ -9058,15 +9058,15 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="29" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
       <c r="D42" s="29" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F42" s="29" t="s">
         <v>65</v>
@@ -9084,15 +9084,15 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="29" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
       <c r="D43" s="29" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F43" s="29" t="s">
         <v>65</v>
@@ -9110,15 +9110,15 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="29" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F44" s="29" t="s">
         <v>65</v>
@@ -9135,15 +9135,15 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="29" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>65</v>
@@ -9160,15 +9160,15 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="29" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
       <c r="D46" s="29" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>65</v>
@@ -9185,15 +9185,15 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="29" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
       <c r="D47" s="29" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>65</v>
@@ -9210,15 +9210,15 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="29" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
       <c r="D48" s="29" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F48" s="29" t="s">
         <v>65</v>
@@ -9235,15 +9235,15 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="29" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
       <c r="D49" s="29" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>65</v>
@@ -9260,15 +9260,15 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="29" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B50" s="29"/>
       <c r="C50" s="29"/>
       <c r="D50" s="29" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F50" s="29" t="s">
         <v>65</v>
@@ -9285,15 +9285,15 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="29" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="29"/>
       <c r="D51" s="29" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F51" s="29" t="s">
         <v>65</v>
@@ -9310,15 +9310,15 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="29" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B52" s="29"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F52" s="29" t="s">
         <v>65</v>
@@ -9335,15 +9335,15 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="29" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B53" s="29"/>
       <c r="C53" s="29"/>
       <c r="D53" s="29" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F53" s="29" t="s">
         <v>64</v>
@@ -9360,15 +9360,15 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="29" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B54" s="29"/>
       <c r="C54" s="29"/>
       <c r="D54" s="29" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F54" s="29" t="s">
         <v>64</v>
@@ -9385,15 +9385,15 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="29" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="29"/>
       <c r="D55" s="29" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F55" s="29" t="s">
         <v>65</v>
@@ -9410,12 +9410,12 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="29" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
       <c r="D56" s="29" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="29" t="s">
@@ -9433,15 +9433,15 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="29" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B57" s="29"/>
       <c r="C57" s="29"/>
       <c r="D57" s="29" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F57" s="29" t="s">
         <v>65</v>
@@ -9458,15 +9458,15 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="29" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
       <c r="D58" s="29" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F58" s="29" t="s">
         <v>65</v>
@@ -9483,15 +9483,15 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="29" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="29"/>
       <c r="D59" s="29" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F59" s="29" t="s">
         <v>65</v>
@@ -9508,15 +9508,15 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="29" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
       <c r="D60" s="29" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F60" s="29" t="s">
         <v>65</v>
@@ -9533,12 +9533,12 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="29" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
       <c r="D61" s="29" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="29" t="s">
@@ -9556,12 +9556,12 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="29" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B62" s="29"/>
       <c r="C62" s="29"/>
       <c r="D62" s="29" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="29" t="s">
@@ -9579,15 +9579,15 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="29" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B63" s="29"/>
       <c r="C63" s="29"/>
       <c r="D63" s="29" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F63" s="29" t="s">
         <v>65</v>
@@ -9604,15 +9604,15 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="29" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
       <c r="D64" s="29" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F64" s="29" t="s">
         <v>65</v>
@@ -9629,15 +9629,15 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="29" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B65" s="29"/>
       <c r="C65" s="29"/>
       <c r="D65" s="29" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F65" s="29" t="s">
         <v>65</v>
@@ -9654,15 +9654,15 @@
     </row>
     <row r="66" spans="1:9" ht="18" customHeight="1">
       <c r="A66" s="29" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B66" s="29"/>
       <c r="C66" s="29"/>
       <c r="D66" s="29" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F66" s="29" t="s">
         <v>65</v>
@@ -9679,15 +9679,15 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="29" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B67" s="29"/>
       <c r="C67" s="29"/>
       <c r="D67" s="29" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F67" s="29" t="s">
         <v>65</v>
@@ -9704,15 +9704,15 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="29" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B68" s="29"/>
       <c r="C68" s="29"/>
       <c r="D68" s="29" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F68" s="29" t="s">
         <v>65</v>
@@ -9729,14 +9729,14 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="29" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B69" s="29"/>
       <c r="D69" s="29" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F69" s="29" t="s">
         <v>65</v>
@@ -9753,14 +9753,14 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="29" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B70" s="29"/>
       <c r="D70" s="29" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F70" s="29" t="s">
         <v>65</v>
@@ -9777,11 +9777,11 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="29" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B71" s="29"/>
       <c r="D71" s="29" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29" t="s">
@@ -9799,14 +9799,14 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="29" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B72" s="29"/>
       <c r="D72" s="29" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F72" s="29" t="s">
         <v>65</v>
@@ -9823,11 +9823,11 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="29" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B73" s="29"/>
       <c r="D73" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E73" s="29"/>
       <c r="F73" s="29" t="s">
@@ -9845,14 +9845,14 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="29" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B74" s="29"/>
       <c r="D74" s="29" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F74" s="29" t="s">
         <v>65</v>
@@ -9869,14 +9869,14 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="29" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B75" s="29"/>
       <c r="D75" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F75" s="29" t="s">
         <v>65</v>
@@ -9893,14 +9893,14 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="29" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B76" s="29"/>
       <c r="D76" s="29" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F76" s="29" t="s">
         <v>65</v>
@@ -9917,14 +9917,14 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B77" s="29"/>
       <c r="D77" s="29" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F77" s="29" t="s">
         <v>65</v>
@@ -9941,14 +9941,14 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B78" s="29"/>
       <c r="D78" s="29" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F78" s="29" t="s">
         <v>65</v>
@@ -9965,14 +9965,14 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="29" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B79" s="29"/>
       <c r="D79" s="29" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F79" s="29" t="s">
         <v>65</v>
@@ -9989,14 +9989,14 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="29" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B80" s="29"/>
       <c r="D80" s="29" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F80" s="29" t="s">
         <v>65</v>
@@ -10013,11 +10013,11 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="29" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B81" s="29"/>
       <c r="D81" s="29" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E81" s="29"/>
       <c r="F81" s="29" t="s">
@@ -10035,14 +10035,14 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="29" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B82" s="29"/>
       <c r="D82" s="29" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F82" s="29" t="s">
         <v>65</v>
@@ -10059,11 +10059,11 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="29" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B83" s="29"/>
       <c r="D83" s="29" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E83" s="29"/>
       <c r="F83" s="29" t="s">
@@ -10081,14 +10081,14 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="29" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B84" s="29"/>
       <c r="D84" s="29" t="s">
+        <v>745</v>
+      </c>
+      <c r="E84" s="29" t="s">
         <v>746</v>
-      </c>
-      <c r="E84" s="29" t="s">
-        <v>747</v>
       </c>
       <c r="F84" s="29" t="s">
         <v>65</v>
@@ -10105,14 +10105,14 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="29" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B85" s="29"/>
       <c r="D85" s="29" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F85" s="29" t="s">
         <v>65</v>
@@ -10129,14 +10129,14 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="29" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B86" s="29"/>
       <c r="D86" s="29" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F86" s="29" t="s">
         <v>65</v>
@@ -10153,14 +10153,14 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B87" s="29"/>
       <c r="D87" s="29" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F87" s="29" t="s">
         <v>65</v>
@@ -10177,14 +10177,14 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B88" s="29"/>
       <c r="D88" s="29" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F88" s="29" t="s">
         <v>65</v>
@@ -10201,14 +10201,14 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="29" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B89" s="29"/>
       <c r="D89" s="29" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F89" s="29" t="s">
         <v>65</v>
@@ -10225,14 +10225,14 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="29" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B90" s="29"/>
       <c r="D90" s="29" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E90" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F90" s="29" t="s">
         <v>65</v>
@@ -10249,14 +10249,14 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="29" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B91" s="29"/>
       <c r="D91" s="29" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E91" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F91" s="29" t="s">
         <v>65</v>
@@ -10273,14 +10273,14 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="29" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B92" s="29"/>
       <c r="D92" s="29" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E92" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F92" s="29" t="s">
         <v>65</v>
@@ -10297,14 +10297,14 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="29" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B93" s="29"/>
       <c r="D93" s="29" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E93" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F93" s="29" t="s">
         <v>65</v>
@@ -10321,14 +10321,14 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="29" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B94" s="29"/>
       <c r="D94" s="29" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E94" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F94" s="29" t="s">
         <v>65</v>
@@ -10345,14 +10345,14 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="29" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B95" s="29"/>
       <c r="D95" s="29" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E95" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F95" s="29" t="s">
         <v>65</v>
@@ -10369,14 +10369,14 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="29" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B96" s="29"/>
       <c r="D96" s="29" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E96" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F96" s="29" t="s">
         <v>65</v>

</xml_diff>